<commit_message>
`UI`: Adjust login & main UI
</commit_message>
<xml_diff>
--- a/src/UI/main/ts/translation.xlsx
+++ b/src/UI/main/ts/translation.xlsx
@@ -2,58 +2,395 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="25600" windowHeight="10500" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="24">
     <font>
       <name val="宋体"/>
       <charset val="1"/>
-      <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <name val="宋体"/>
+      <charset val="1"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="宋体"/>
       <charset val="134"/>
-      <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="35">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -62,7 +399,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -70,46 +407,516 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <horizontal style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7">
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+    </tableStyle>
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10">
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -182,41 +989,41 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
     <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1f497d"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="eeece1"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4f81bd"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="c0504d"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9bbb59"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064a2"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4bacc6"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="f79646"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ff"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -224,17 +1031,17 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme>
+    <a:fmtScheme name="">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -258,7 +1065,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -279,7 +1086,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -330,7 +1137,7 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -348,388 +1155,425 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.61328125" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.61363636363636" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1" s="3">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1" ht="14.25" customHeight="1" s="2">
+      <c r="A1" t="inlineStr">
         <is>
           <t>code:</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>zh-CHS</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>en</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>zh-CHT</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>fr</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>ko</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>ja</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1" s="3">
-      <c r="A2" s="4" t="inlineStr">
+    <row r="2" ht="14.25" customHeight="1" s="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>MainWindow</t>
         </is>
       </c>
-      <c r="B2" s="4" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>主窗口</t>
         </is>
       </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>MainWindow</t>
         </is>
       </c>
-      <c r="D2" s="4" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>主視窗</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>메인윈도우</t>
         </is>
       </c>
-      <c r="G2" s="4" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>メインウィンドウ</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1" s="3">
-      <c r="A3" s="4" t="inlineStr">
+    <row r="3" ht="14.25" customHeight="1" s="2">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Frame</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>框架</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Frame</t>
         </is>
       </c>
-      <c r="D3" s="4" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>框架</t>
         </is>
       </c>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="F3" s="4" t="inlineStr">
         <is>
           <t>프레임</t>
         </is>
       </c>
-      <c r="G3" s="4" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>フレーム</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1" s="3">
-      <c r="A4" s="4" t="inlineStr">
+    <row r="4" ht="14.25" customHeight="1" s="2">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Exit</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>退出</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Exit</t>
         </is>
       </c>
-      <c r="D4" s="4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>退出</t>
         </is>
       </c>
-      <c r="F4" s="5" t="inlineStr">
+      <c r="F4" s="4" t="inlineStr">
         <is>
           <t>출구</t>
         </is>
       </c>
-      <c r="G4" s="4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>出口</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1" s="3">
-      <c r="A5" s="4" t="inlineStr">
+    <row r="5" ht="14.25" customHeight="1" s="2">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Show</t>
         </is>
       </c>
-      <c r="B5" s="4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>显示</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Show</t>
         </is>
       </c>
-      <c r="D5" s="4" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>顯示</t>
         </is>
       </c>
-      <c r="F5" s="5" t="inlineStr">
+      <c r="F5" s="4" t="inlineStr">
         <is>
           <t>보이다</t>
         </is>
       </c>
-      <c r="G5" s="4" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>見せる</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1" s="3">
-      <c r="A6" s="6" t="inlineStr">
+    <row r="6" ht="14.25" customHeight="1" s="2">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>Message</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>消息</t>
         </is>
       </c>
-      <c r="C6" s="4" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Message</t>
         </is>
       </c>
-      <c r="D6" s="4" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>消息</t>
         </is>
       </c>
-      <c r="F6" s="5" t="inlineStr">
+      <c r="F6" s="4" t="inlineStr">
         <is>
           <t>메시지</t>
         </is>
       </c>
-      <c r="G6" s="4" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>メッセージ</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1" s="3">
-      <c r="A7" s="4" t="inlineStr">
+    <row r="7" ht="14.25" customHeight="1" s="2">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Setting</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>设置</t>
         </is>
       </c>
-      <c r="C7" s="4" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Setting</t>
         </is>
       </c>
-      <c r="D7" s="4" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>設置</t>
         </is>
       </c>
-      <c r="F7" s="5" t="inlineStr">
+      <c r="F7" s="4" t="inlineStr">
         <is>
           <t>설정</t>
         </is>
       </c>
-      <c r="G7" s="4" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>設定</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1" s="3">
-      <c r="A8" s="6" t="inlineStr">
+    <row r="8" ht="14.25" customHeight="1" s="2">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>Work platform</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>工作平台</t>
         </is>
       </c>
-      <c r="C8" s="4" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Work platform</t>
         </is>
       </c>
-      <c r="D8" s="4" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>工作平臺</t>
         </is>
       </c>
-      <c r="F8" s="5" t="inlineStr">
+      <c r="F8" s="4" t="inlineStr">
         <is>
           <t>작업 플랫폼</t>
         </is>
       </c>
-      <c r="G8" s="4" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>作業プラットフォーム</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1" s="3">
-      <c r="A9" s="6" t="inlineStr">
+    <row r="9" ht="14.25" customHeight="1" s="2">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>Meeting</t>
         </is>
       </c>
-      <c r="B9" s="4" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>会议</t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Meeting</t>
         </is>
       </c>
-      <c r="D9" s="4" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>會議</t>
         </is>
       </c>
-      <c r="F9" s="5" t="inlineStr">
+      <c r="F9" s="4" t="inlineStr">
         <is>
           <t>회의</t>
         </is>
       </c>
-      <c r="G9" s="4" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>会議</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1" s="3">
-      <c r="A10" s="6" t="inlineStr">
+    <row r="10" ht="14.25" customHeight="1" s="2">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>Classroom</t>
         </is>
       </c>
-      <c r="B10" s="4" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>课堂</t>
         </is>
       </c>
-      <c r="C10" s="4" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Classroom</t>
         </is>
       </c>
-      <c r="D10" s="4" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>課堂</t>
         </is>
       </c>
-      <c r="F10" s="4" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>교실</t>
         </is>
       </c>
-      <c r="G10" s="4" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>教室</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1" s="3">
-      <c r="A11" s="6" t="inlineStr">
+    <row r="11" ht="14.25" customHeight="1" s="2">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>Document</t>
         </is>
       </c>
-      <c r="B11" s="4" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>文档</t>
         </is>
       </c>
-      <c r="C11" s="4" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Document</t>
         </is>
       </c>
-      <c r="D11" s="4" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>文件</t>
         </is>
       </c>
-      <c r="F11" s="4" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>문서조사</t>
         </is>
       </c>
-      <c r="G11" s="4" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>文書</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>登录</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Sign in</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>登錄</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Connexion</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>로그인</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>ログイン</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>